<commit_message>
plotted all p-persistent graphs
</commit_message>
<xml_diff>
--- a/p-persistent results.xlsx
+++ b/p-persistent results.xlsx
@@ -37,7 +37,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -61,8 +61,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -73,6 +80,12 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6B8B7"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -94,20 +107,43 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -170,7 +206,96 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:f>Sheet1!$B$12:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$32:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>8.64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35.52</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41.16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>47.88</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>55.44</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>69.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>P = 0.01</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$12:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -214,34 +339,223 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8.64</c:v>
+                  <c:v>6.96</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34.68</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.92</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50.04</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>68.16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>P = 0.1</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$12:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$12:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>7.68</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.44</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.68</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36.84</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42.48</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>49.56</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>58.44</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64.56</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>68.64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>P = 0.3</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$22:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6.48</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>13.92</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.36</c:v>
+                  <c:v>20.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26.4</c:v>
+                  <c:v>26.64</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.52</c:v>
+                  <c:v>34.08</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41.16</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>47.88</c:v>
+                  <c:v>48.84</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>55.44</c:v>
+                  <c:v>59.28</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>66.0</c:v>
+                  <c:v>63.72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>69.12</c:v>
+                  <c:v>71.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>P = 1.0</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$42:$C$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.68</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.52</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35.16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44.28</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>48.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>55.92</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>65.16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>67.08</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -258,11 +572,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2141486856"/>
-        <c:axId val="2141692168"/>
+        <c:axId val="2145945384"/>
+        <c:axId val="2139671224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2141486856"/>
+        <c:axId val="2145945384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -291,7 +605,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141692168"/>
+        <c:crossAx val="2139671224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -299,7 +613,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2141692168"/>
+        <c:axId val="2139671224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -329,7 +643,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141486856"/>
+        <c:crossAx val="2145945384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -406,7 +720,96 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:f>Sheet1!$B$42:$B$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$32:$D$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>306149.805556</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>411893.956897</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>399379.921348</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>453533.772727</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>453624.780405</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>456738.921283</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>457213.674185</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>480637.324675</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>480155.863636</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>486248.201389</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>P = 0.01</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$42:$B$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -450,34 +853,301 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>306149.805556</c:v>
+                  <c:v>247504.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>411893.956897</c:v>
+                  <c:v>436864.491071</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>399379.921348</c:v>
+                  <c:v>439096.038889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>453533.772727</c:v>
+                  <c:v>437659.547009</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>453624.780405</c:v>
+                  <c:v>458496.155709</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>456738.921283</c:v>
+                  <c:v>461148.504399</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>457213.674185</c:v>
+                  <c:v>469800.153477</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>480637.324675</c:v>
+                  <c:v>479186.873333</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>480155.863636</c:v>
+                  <c:v>477472.605825</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>486248.201389</c:v>
+                  <c:v>488558.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>P = 0.1</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$42:$B$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$12:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>215196.90625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>397046.050847</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>438044.989305</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>423940.627615</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>473015.234528</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>468841.748588</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>463746.27845</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>490530.876797</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>467093.907063</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>477422.243007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>P = 0.3</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$42:$B$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$22:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>210039.796296</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>371774.784483</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>452682.964706</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>444140.463964</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>462634.397887</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>483247.18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>468920.36855</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>472225.91498</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>479927.299435</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>488228.215126</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>P = 1.0</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$42:$B$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$42:$D$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>216813.353846</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>407316.184211</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>423702.426901</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>439580.118367</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>448440.627986</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>475121.723577</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>477189.320988</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>484498.300429</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>477870.548803</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>481034.11449</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -494,11 +1164,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2142724232"/>
-        <c:axId val="2142585752"/>
+        <c:axId val="2142472568"/>
+        <c:axId val="2139444728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2142724232"/>
+        <c:axId val="2142472568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -527,7 +1197,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142585752"/>
+        <c:crossAx val="2139444728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -535,10 +1205,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142585752"/>
+        <c:axId val="2139444728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="250000.0"/>
+          <c:min val="200000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -566,7 +1236,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142724232"/>
+        <c:crossAx val="2142472568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -592,16 +1262,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>452438</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>174627</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>363538</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>71438</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>808038</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>73820</xdr:rowOff>
+      <xdr:rowOff>175420</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -622,16 +1292,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>261938</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>96838</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>8759</xdr:rowOff>
+      <xdr:rowOff>135759</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>706438</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>105569</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>541338</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>42069</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -975,10 +1645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1004,16 +1674,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>0.6</v>
+        <v>0.01</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>8.64</v>
+        <v>6.96</v>
       </c>
       <c r="D2" s="1">
-        <v>306149.80555599998</v>
+        <v>247504.5</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1021,10 +1691,10 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>13.92</v>
+        <v>13.44</v>
       </c>
       <c r="D3">
-        <v>411893.95689700003</v>
+        <v>436864.491071</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1032,10 +1702,10 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>21.36</v>
+        <v>21.6</v>
       </c>
       <c r="D4">
-        <v>399379.921348</v>
+        <v>439096.03888900002</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1043,10 +1713,10 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>26.4</v>
+        <v>28.08</v>
       </c>
       <c r="D5">
-        <v>453533.772727</v>
+        <v>437659.54700899997</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1054,10 +1724,10 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>35.520000000000003</v>
+        <v>34.68</v>
       </c>
       <c r="D6">
-        <v>453624.78040500003</v>
+        <v>458496.15570900001</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1065,10 +1735,10 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>41.16</v>
+        <v>40.92</v>
       </c>
       <c r="D7">
-        <v>456738.92128299997</v>
+        <v>461148.50439900003</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1076,10 +1746,10 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>47.88</v>
+        <v>50.04</v>
       </c>
       <c r="D8">
-        <v>457213.67418500001</v>
+        <v>469800.15347700001</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1087,10 +1757,10 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>55.44</v>
+        <v>54</v>
       </c>
       <c r="D9">
-        <v>480637.32467499998</v>
+        <v>479186.873333</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1098,10 +1768,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>66</v>
+        <v>61.8</v>
       </c>
       <c r="D10">
-        <v>480155.86363600002</v>
+        <v>477472.60582499998</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1109,14 +1779,541 @@
         <v>10</v>
       </c>
       <c r="C11">
+        <v>68.16</v>
+      </c>
+      <c r="D11">
+        <v>488558.125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>7.68</v>
+      </c>
+      <c r="D12" s="1">
+        <v>215196.90625</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>14.16</v>
+      </c>
+      <c r="D13">
+        <v>397046.05084699998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>22.44</v>
+      </c>
+      <c r="D14">
+        <v>438044.989305</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15" s="3">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>28.68</v>
+      </c>
+      <c r="D15">
+        <v>423940.627615</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="D16">
+        <v>473015.234528</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>42.48</v>
+      </c>
+      <c r="D17">
+        <v>468841.74858800002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="B18" s="3">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>49.56</v>
+      </c>
+      <c r="D18">
+        <v>463746.27844999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>58.44</v>
+      </c>
+      <c r="D19">
+        <v>490530.876797</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>64.56</v>
+      </c>
+      <c r="D20">
+        <v>467093.90706300002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="B21" s="3">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>68.64</v>
+      </c>
+      <c r="D21">
+        <v>477422.24300700001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1">
+        <v>6.48</v>
+      </c>
+      <c r="D22" s="1">
+        <v>210039.79629599999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>13.92</v>
+      </c>
+      <c r="D23">
+        <v>371774.784483</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D24">
+        <v>452682.964706</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>26.64</v>
+      </c>
+      <c r="D25">
+        <v>444140.463964</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>34.08</v>
+      </c>
+      <c r="D26">
+        <v>462634.397887</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6">
+        <v>6</v>
+      </c>
+      <c r="C27">
+        <v>42</v>
+      </c>
+      <c r="D27">
+        <v>483247.18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>48.84</v>
+      </c>
+      <c r="D28">
+        <v>468920.36855000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>59.28</v>
+      </c>
+      <c r="D29">
+        <v>472225.91498</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6">
+        <v>9</v>
+      </c>
+      <c r="C30">
+        <v>63.72</v>
+      </c>
+      <c r="D30">
+        <v>479927.29943499999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6">
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="D31">
+        <v>488228.215126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1">
+        <v>8.64</v>
+      </c>
+      <c r="D32" s="1">
+        <v>306149.80555599998</v>
+      </c>
+      <c r="E32">
+        <v>7.68</v>
+      </c>
+      <c r="F32">
+        <v>303769.703125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>13.92</v>
+      </c>
+      <c r="D33">
+        <v>411893.95689700003</v>
+      </c>
+      <c r="E33">
+        <v>13.68</v>
+      </c>
+      <c r="F33">
+        <v>422658.84210499999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>21.36</v>
+      </c>
+      <c r="D34">
+        <v>399379.921348</v>
+      </c>
+      <c r="E34">
+        <v>19.8</v>
+      </c>
+      <c r="F34">
+        <v>404839.85454500001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="B35" s="3">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>26.4</v>
+      </c>
+      <c r="D35">
+        <v>453533.772727</v>
+      </c>
+      <c r="E35">
+        <v>27.48</v>
+      </c>
+      <c r="F35">
+        <v>461375.17030599999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36">
+        <v>35.520000000000003</v>
+      </c>
+      <c r="D36">
+        <v>453624.78040500003</v>
+      </c>
+      <c r="E36">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="F36">
+        <v>468233.92580600001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="B37">
+        <v>6</v>
+      </c>
+      <c r="C37">
+        <v>41.16</v>
+      </c>
+      <c r="D37">
+        <v>456738.92128299997</v>
+      </c>
+      <c r="E37">
+        <v>41.4</v>
+      </c>
+      <c r="F37">
+        <v>468102.05507200002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="B38" s="3">
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <v>47.88</v>
+      </c>
+      <c r="D38">
+        <v>457213.67418500001</v>
+      </c>
+      <c r="E38">
+        <v>50.64</v>
+      </c>
+      <c r="F38">
+        <v>469867.33649299998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="B39">
+        <v>8</v>
+      </c>
+      <c r="C39">
+        <v>55.44</v>
+      </c>
+      <c r="D39">
+        <v>480637.32467499998</v>
+      </c>
+      <c r="E39">
+        <v>57.84</v>
+      </c>
+      <c r="F39">
+        <v>483227.49170100002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="B40">
+        <v>9</v>
+      </c>
+      <c r="C40">
+        <v>66</v>
+      </c>
+      <c r="D40">
+        <v>480155.86363600002</v>
+      </c>
+      <c r="E40">
+        <v>61.08</v>
+      </c>
+      <c r="F40">
+        <v>478224.71316300001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="B41" s="3">
+        <v>10</v>
+      </c>
+      <c r="C41">
         <v>69.12</v>
       </c>
-      <c r="D11">
+      <c r="D41">
         <v>486248.20138899999</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="B12" s="3"/>
+      <c r="E41">
+        <v>71.16</v>
+      </c>
+      <c r="F41">
+        <v>483271.98650900001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="4">
+        <v>1</v>
+      </c>
+      <c r="B42" s="5">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1">
+        <v>7.8</v>
+      </c>
+      <c r="D42" s="1">
+        <v>216813.35384600001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>13.68</v>
+      </c>
+      <c r="D43">
+        <v>407316.18421099999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>20.52</v>
+      </c>
+      <c r="D44">
+        <v>423702.42690100003</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>29.4</v>
+      </c>
+      <c r="D45">
+        <v>439580.11836700002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>35.159999999999997</v>
+      </c>
+      <c r="D46">
+        <v>448440.62798599998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6">
+        <v>6</v>
+      </c>
+      <c r="C47">
+        <v>44.28</v>
+      </c>
+      <c r="D47">
+        <v>475121.72357700003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6">
+        <v>7</v>
+      </c>
+      <c r="C48">
+        <v>48.6</v>
+      </c>
+      <c r="D48">
+        <v>477189.32098800002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6">
+        <v>8</v>
+      </c>
+      <c r="C49">
+        <v>55.92</v>
+      </c>
+      <c r="D49">
+        <v>484498.300429</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6">
+        <v>9</v>
+      </c>
+      <c r="C50">
+        <v>65.16</v>
+      </c>
+      <c r="D50">
+        <v>477870.54880300001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6">
+        <v>10</v>
+      </c>
+      <c r="C51">
+        <v>67.08</v>
+      </c>
+      <c r="D51">
+        <v>481034.11449000001</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>